<commit_message>
Adding sheets 2 and 3 that contains planning for Sprint 1 User stories
</commit_message>
<xml_diff>
--- a/Details.xlsx
+++ b/Details.xlsx
@@ -1,20 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shubh\CS555-AgileProject\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4157F9F-954D-44D6-BC65-2A87DF66F178}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="14355" windowHeight="8775"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="73">
   <si>
     <t>Coding</t>
   </si>
@@ -166,14 +177,80 @@
     <t xml:space="preserve">Initial </t>
   </si>
   <si>
-    <t>CS555-AgileProject-Group22</t>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Remaining Stories</t>
+  </si>
+  <si>
+    <t>Story Velocity</t>
+  </si>
+  <si>
+    <t>LOC</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Code Velocity</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    03-01-2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    03-17-2021</t>
+  </si>
+  <si>
+    <t>Est Size</t>
+  </si>
+  <si>
+    <t>Est Time</t>
+  </si>
+  <si>
+    <t>Act Size</t>
+  </si>
+  <si>
+    <t>Act Time</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Dates before current date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Birth before marriage </t>
+  </si>
+  <si>
+    <t>US03</t>
+  </si>
+  <si>
+    <t>Birth before death</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US07 </t>
+  </si>
+  <si>
+    <t>Less then 150 years old</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Birth before marriage of parents </t>
+  </si>
+  <si>
+    <t>CS555-AgileProject-Group2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -301,7 +378,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -324,6 +401,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -331,7 +412,1865 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>BURN DOWN chart</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[1]Sheet2!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Remaining Stories</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>[1]Sheet2!$B$4:$C$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>[1]Sheet2!$B$4:$C$4</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="1"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>    03-01-2021</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Start</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>[1]Sheet2!$D$4:$D$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>[1]Sheet2!$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-67FE-497C-B527-7002BAAE672A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="561652904"/>
+        <c:axId val="561653888"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>[1]Sheet2!$E$3</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Story Velocity</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="22225" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="square"/>
+                  <c:size val="6"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="50000"/>
+                              <a:lumOff val="50000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="t"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:multiLvlStrRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>[1]Sheet2!$B$4:$C$5</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>[1]Sheet2!$B$4:$C$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:multiLvlStrCache>
+                      <c:ptCount val="1"/>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>    03-01-2021</c:v>
+                        </c:pt>
+                      </c:lvl>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>Start</c:v>
+                        </c:pt>
+                      </c:lvl>
+                    </c:multiLvlStrCache>
+                  </c:multiLvlStrRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>[1]Sheet2!$E$4:$E$5</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>[1]Sheet2!$E$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="1"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-67FE-497C-B527-7002BAAE672A}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>[1]Sheet2!$F$3</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>LOC</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="22225" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="triangle"/>
+                  <c:size val="6"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3"/>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="50000"/>
+                              <a:lumOff val="50000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="t"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:multiLvlStrRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>[1]Sheet2!$B$4:$C$5</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>[1]Sheet2!$B$4:$C$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:multiLvlStrCache>
+                      <c:ptCount val="1"/>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>    03-01-2021</c:v>
+                        </c:pt>
+                      </c:lvl>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>Start</c:v>
+                        </c:pt>
+                      </c:lvl>
+                    </c:multiLvlStrCache>
+                  </c:multiLvlStrRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>[1]Sheet2!$F$4:$F$5</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>[1]Sheet2!$F$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-67FE-497C-B527-7002BAAE672A}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>[1]Sheet2!$G$3</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Min</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="22225" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="x"/>
+                  <c:size val="6"/>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent4"/>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="50000"/>
+                              <a:lumOff val="50000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="t"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:multiLvlStrRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>[1]Sheet2!$B$4:$C$5</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>[1]Sheet2!$B$4:$C$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:multiLvlStrCache>
+                      <c:ptCount val="1"/>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>    03-01-2021</c:v>
+                        </c:pt>
+                      </c:lvl>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>Start</c:v>
+                        </c:pt>
+                      </c:lvl>
+                    </c:multiLvlStrCache>
+                  </c:multiLvlStrRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>[1]Sheet2!$G$4:$G$5</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>[1]Sheet2!$G$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="1"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-67FE-497C-B527-7002BAAE672A}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="4"/>
+                <c:order val="4"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>[1]Sheet2!$H$3</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Code Velocity</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="22225" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent5"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="star"/>
+                  <c:size val="6"/>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent5"/>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="50000"/>
+                              <a:lumOff val="50000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="t"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:multiLvlStrRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>[1]Sheet2!$B$4:$C$5</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>[1]Sheet2!$B$4:$C$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:multiLvlStrCache>
+                      <c:ptCount val="1"/>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>    03-01-2021</c:v>
+                        </c:pt>
+                      </c:lvl>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>Start</c:v>
+                        </c:pt>
+                      </c:lvl>
+                    </c:multiLvlStrCache>
+                  </c:multiLvlStrRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>[1]Sheet2!$H$4:$H$5</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>[1]Sheet2!$H$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="1"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000004-67FE-497C-B527-7002BAAE672A}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="561652904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN"/>
+                  <a:t>dates</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="561653888"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="561653888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN" baseline="0"/>
+                  <a:t>rEMAINING stories</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-IN"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.6666666666666666E-2"/>
+              <c:y val="0.30253827646544185"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="561652904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="239">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>396875</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>92075</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>73025</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DD35CEC-24C0-4E18-8138-631ACCAB9487}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet2"/>
+      <sheetName val="Sheet3"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="D3" t="str">
+            <v>Remaining Stories</v>
+          </cell>
+          <cell r="E3" t="str">
+            <v>Story Velocity</v>
+          </cell>
+          <cell r="F3" t="str">
+            <v>LOC</v>
+          </cell>
+          <cell r="G3" t="str">
+            <v>Min</v>
+          </cell>
+          <cell r="H3" t="str">
+            <v>Code Velocity</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4" t="str">
+            <v>Start</v>
+          </cell>
+          <cell r="C4" t="str">
+            <v xml:space="preserve">    03-01-2021</v>
+          </cell>
+          <cell r="D4">
+            <v>32</v>
+          </cell>
+          <cell r="F4">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5" t="str">
+            <v xml:space="preserve">Sprint 1 </v>
+          </cell>
+          <cell r="C5" t="str">
+            <v xml:space="preserve">    03-17-2021</v>
+          </cell>
+          <cell r="D5">
+            <v>24</v>
+          </cell>
+          <cell r="E5">
+            <v>8</v>
+          </cell>
+          <cell r="F5">
+            <v>240</v>
+          </cell>
+          <cell r="G5">
+            <v>480</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -377,7 +2316,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -409,9 +2348,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -443,6 +2400,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -618,22 +2593,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" customWidth="1"/>
+    <col min="3" max="4" width="11.1796875" customWidth="1"/>
+    <col min="5" max="5" width="29.1796875" customWidth="1"/>
+    <col min="6" max="6" width="27.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:6">
+    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B2" s="12" t="s">
         <v>49</v>
       </c>
@@ -650,7 +2625,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="2:6">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" s="8" t="s">
         <v>19</v>
       </c>
@@ -667,7 +2642,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="2:6">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B4" s="8" t="s">
         <v>2</v>
       </c>
@@ -684,7 +2659,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" s="8" t="s">
         <v>7</v>
       </c>
@@ -701,7 +2676,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B6" s="8" t="s">
         <v>16</v>
       </c>
@@ -718,7 +2693,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" s="8"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -726,17 +2701,17 @@
         <v>28</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="15.75" thickBot="1">
+    <row r="8" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="4"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="11" spans="2:6">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>27</v>
       </c>
@@ -753,7 +2728,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="2:6">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>1</v>
       </c>
@@ -770,7 +2745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:6">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B13">
         <v>1</v>
       </c>
@@ -787,7 +2762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:6">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B14">
         <v>1</v>
       </c>
@@ -804,7 +2779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:6">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B15">
         <v>1</v>
       </c>
@@ -821,7 +2796,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="2:6">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B16">
         <v>1</v>
       </c>
@@ -838,7 +2813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17">
         <v>1</v>
       </c>
@@ -855,7 +2830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18">
         <v>1</v>
       </c>
@@ -872,7 +2847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B19">
         <v>1</v>
       </c>
@@ -891,12 +2866,305 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E6" r:id="rId1"/>
-    <hyperlink ref="E5" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
-    <hyperlink ref="E3" r:id="rId4"/>
+    <hyperlink ref="E6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9A4E240-DEFC-434E-B354-C03F0C5A68FC}">
+  <dimension ref="D5:K7"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" width="12.453125" customWidth="1"/>
+    <col min="6" max="6" width="19.26953125" customWidth="1"/>
+    <col min="7" max="7" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="D5" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="D6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6">
+        <v>32</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="D7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F7">
+        <v>24</v>
+      </c>
+      <c r="G7">
+        <v>8</v>
+      </c>
+      <c r="H7">
+        <v>240</v>
+      </c>
+      <c r="I7">
+        <v>480</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA93B4A9-22E1-4762-8978-87F966DD9584}">
+  <dimension ref="D3:L11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" width="32.08984375" customWidth="1"/>
+    <col min="8" max="8" width="9.81640625" customWidth="1"/>
+    <col min="9" max="9" width="9.7265625" customWidth="1"/>
+    <col min="10" max="10" width="9.26953125" customWidth="1"/>
+    <col min="11" max="11" width="9.453125" customWidth="1"/>
+    <col min="12" max="12" width="13.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>30</v>
+      </c>
+      <c r="I4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>30</v>
+      </c>
+      <c r="I5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>30</v>
+      </c>
+      <c r="I6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>30</v>
+      </c>
+      <c r="I7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>30</v>
+      </c>
+      <c r="I8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>30</v>
+      </c>
+      <c r="I9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>30</v>
+      </c>
+      <c r="I10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>30</v>
+      </c>
+      <c r="I11">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>